<commit_message>
adding rapid transect data plus tests
</commit_message>
<xml_diff>
--- a/data/raw/PinellasCo20210404.xlsx
+++ b/data/raw/PinellasCo20210404.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\proj\piney-point\data\stations\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\proj\piney-point\data\raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1BA6CA3F-A41F-4FEA-99A7-C0AF67F77826}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74ACD32A-962F-4A12-BB75-3F9D269E9781}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30675" yWindow="2880" windowWidth="19905" windowHeight="9600" xr2:uid="{7CCBBE23-BA76-4D5F-AE25-A63AE4902556}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{7CCBBE23-BA76-4D5F-AE25-A63AE4902556}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -436,7 +436,7 @@
   <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="A10" sqref="A10:XFD10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>